<commit_message>
Gihyen Eom - ge2247
</commit_message>
<xml_diff>
--- a/final.xlsx
+++ b/final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal2222\source\repos\keithalewis\final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\source\repos\final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDECEC16-5D22-4C9F-9072-BB4EA1AA88DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E009E815-C276-433B-AD8B-B6F2599D0FED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3308" yWindow="3308" windowWidth="15390" windowHeight="9982" xr2:uid="{59ABE93D-F590-4F15-A965-72CEF18EA92E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59ABE93D-F590-4F15-A965-72CEF18EA92E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,14 +37,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -477,14 +475,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED1841A-FD92-4362-9698-89095B3322F2}">
   <dimension ref="B2:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.59765625" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,7 +494,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -500,7 +502,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -508,7 +510,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -528,7 +530,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F6" s="3" t="s">
         <v>7</v>
       </c>
@@ -545,7 +547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>4</v>
       </c>
@@ -559,14 +561,20 @@
         <f t="array" ref="G7">_xll.XLL.BLACK.PUT(f, sigma, F7, t)</f>
         <v>3.7401735689890359E-4</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F7,t)</f>
+        <v>8.9763951445043927E-4</v>
+      </c>
       <c r="I7" cm="1">
         <f t="array" ref="I7">_xll.XLL.BLACK.PUT.IMPLIED(f, G7, F7, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="J7" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H7, F7, t)</f>
+        <v>0.21231052715334578</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -574,7 +582,10 @@
         <f t="array" ref="C8">_xll.XLL.BLACK.PUT(f, sigma, k, t)</f>
         <v>3.987761167674492</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,k,t)</f>
+        <v>3.9960690164368557</v>
+      </c>
       <c r="F8">
         <v>71</v>
       </c>
@@ -582,14 +593,20 @@
         <f t="array" ref="G8">_xll.XLL.BLACK.PUT(f, sigma, F8, t)</f>
         <v>6.6190274539823513E-4</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F8,t)</f>
+        <v>1.4575439098829177E-3</v>
+      </c>
       <c r="I8" cm="1">
         <f t="array" ref="I8">_xll.XLL.BLACK.PUT.IMPLIED(f, G8, F8, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="J8" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H8, F8, t)</f>
+        <v>0.21183817179416867</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F9">
         <v>72</v>
       </c>
@@ -597,14 +614,20 @@
         <f t="array" ref="G9">_xll.XLL.BLACK.PUT(f, sigma, F9, t)</f>
         <v>1.1416834541484455E-3</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F9,t)</f>
+        <v>2.3228003245620993E-3</v>
+      </c>
       <c r="I9" cm="1">
         <f t="array" ref="I9">_xll.XLL.BLACK.PUT.IMPLIED(f, G9, F9, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="J9" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H9, F9, t)</f>
+        <v>0.21137234937840421</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F10">
         <v>73</v>
       </c>
@@ -612,14 +635,20 @@
         <f t="array" ref="G10">_xll.XLL.BLACK.PUT(f, sigma, F10, t)</f>
         <v>1.921340827967688E-3</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F10,t)</f>
+        <v>3.6352252638087446E-3</v>
+      </c>
       <c r="I10" cm="1">
         <f t="array" ref="I10">_xll.XLL.BLACK.PUT.IMPLIED(f, G10, F10, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="J10" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H10, F10, t)</f>
+        <v>0.21091288331598537</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F11">
         <v>74</v>
       </c>
@@ -627,14 +656,20 @@
         <f t="array" ref="G11">_xll.XLL.BLACK.PUT(f, sigma, F11, t)</f>
         <v>3.1579703105526491E-3</v>
       </c>
-      <c r="H11" s="2"/>
+      <c r="H11" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F11,t)</f>
+        <v>5.590231529384676E-3</v>
+      </c>
       <c r="I11" cm="1">
         <f t="array" ref="I11">_xll.XLL.BLACK.PUT.IMPLIED(f, G11, F11, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="J11" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H11, F11, t)</f>
+        <v>0.21045960410593448</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F12">
         <v>75</v>
       </c>
@@ -642,14 +677,20 @@
         <f t="array" ref="G12">_xll.XLL.BLACK.PUT(f, sigma, F12, t)</f>
         <v>5.0742901084088743E-3</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F12,t)</f>
+        <v>8.451791248063445E-3</v>
+      </c>
       <c r="I12" cm="1">
         <f t="array" ref="I12">_xll.XLL.BLACK.PUT.IMPLIED(f, G12, F12, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="J12" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H12, F12, t)</f>
+        <v>0.21001234896104137</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F13">
         <v>76</v>
       </c>
@@ -657,14 +698,20 @@
         <f t="array" ref="G13">_xll.XLL.BLACK.PUT(f, sigma, F13, t)</f>
         <v>7.978238008985894E-3</v>
       </c>
-      <c r="H13" s="2"/>
+      <c r="H13" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F13,t)</f>
+        <v>1.2569613235804633E-2</v>
+      </c>
       <c r="I13" cm="1">
         <f t="array" ref="I13">_xll.XLL.BLACK.PUT.IMPLIED(f, G13, F13, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="J13" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H13, F13, t)</f>
+        <v>0.20957096145645532</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F14">
         <v>77</v>
       </c>
@@ -672,14 +719,20 @@
         <f t="array" ref="G14">_xll.XLL.BLACK.PUT(f, sigma, F14, t)</f>
         <v>1.228534023985528E-2</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F14,t)</f>
+        <v>1.8398212800229241E-2</v>
+      </c>
       <c r="I14" cm="1">
         <f t="array" ref="I14">_xll.XLL.BLACK.PUT.IMPLIED(f, G14, F14, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="J14" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H14, F14, t)</f>
+        <v>0.20913529120173258</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F15">
         <v>78</v>
       </c>
@@ -687,14 +740,20 @@
         <f t="array" ref="G15">_xll.XLL.BLACK.PUT(f, sigma, F15, t)</f>
         <v>1.8543180097092993E-2</v>
       </c>
-      <c r="H15" s="2"/>
+      <c r="H15" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F15,t)</f>
+        <v>2.6517310308358133E-2</v>
+      </c>
       <c r="I15" cm="1">
         <f t="array" ref="I15">_xll.XLL.BLACK.PUT.IMPLIED(f, G15, F15, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="J15" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H15, F15, t)</f>
+        <v>0.20870519353355413</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F16">
         <v>79</v>
       </c>
@@ -702,14 +761,20 @@
         <f t="array" ref="G16">_xll.XLL.BLACK.PUT(f, sigma, F16, t)</f>
         <v>2.7456906561138417E-2</v>
       </c>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F16,t)</f>
+        <v>3.7652736229766726E-2</v>
+      </c>
       <c r="I16" cm="1">
         <f t="array" ref="I16">_xll.XLL.BLACK.PUT.IMPLIED(f, G16, F16, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J16" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H16, F16, t)</f>
+        <v>0.20828052922744211</v>
+      </c>
+    </row>
+    <row r="17" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F17">
         <v>80</v>
       </c>
@@ -717,14 +782,20 @@
         <f t="array" ref="G17">_xll.XLL.BLACK.PUT(f, sigma, F17, t)</f>
         <v>3.991434342184963E-2</v>
       </c>
-      <c r="H17" s="2"/>
+      <c r="H17" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F17,t)</f>
+        <v>5.2696767052352822E-2</v>
+      </c>
       <c r="I17" cm="1">
         <f t="array" ref="I17">_xll.XLL.BLACK.PUT.IMPLIED(f, G17, F17, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J17" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H17, F17, t)</f>
+        <v>0.20786116422816761</v>
+      </c>
+    </row>
+    <row r="18" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F18">
         <v>81</v>
       </c>
@@ -732,14 +803,20 @@
         <f t="array" ref="G18">_xll.XLL.BLACK.PUT(f, sigma, F18, t)</f>
         <v>5.7008934088089269E-2</v>
       </c>
-      <c r="H18" s="2"/>
+      <c r="H18" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F18,t)</f>
+        <v>7.2726594958209656E-2</v>
+      </c>
       <c r="I18" cm="1">
         <f t="array" ref="I18">_xll.XLL.BLACK.PUT.IMPLIED(f, G18, F18, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J18" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H18, F18, t)</f>
+        <v>0.20744696939560114</v>
+      </c>
+    </row>
+    <row r="19" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F19">
         <v>82</v>
       </c>
@@ -747,14 +824,20 @@
         <f t="array" ref="G19">_xll.XLL.BLACK.PUT(f, sigma, F19, t)</f>
         <v>8.0058534547871929E-2</v>
       </c>
-      <c r="H19" s="2"/>
+      <c r="H19" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F19,t)</f>
+        <v>9.9019472852507118E-2</v>
+      </c>
       <c r="I19" cm="1">
         <f t="array" ref="I19">_xll.XLL.BLACK.PUT.IMPLIED(f, G19, F19, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J19" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H19, F19, t)</f>
+        <v>0.20703782026762049</v>
+      </c>
+    </row>
+    <row r="20" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F20">
         <v>83</v>
       </c>
@@ -762,14 +845,20 @@
         <f t="array" ref="G20">_xll.XLL.BLACK.PUT(f, sigma, F20, t)</f>
         <v>0.1106179901946911</v>
       </c>
-      <c r="H20" s="2"/>
+      <c r="H20" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F20,t)</f>
+        <v>0.13306300235605129</v>
+      </c>
       <c r="I20" cm="1">
         <f t="array" ref="I20">_xll.XLL.BLACK.PUT.IMPLIED(f, G20, F20, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J20" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H20, F20, t)</f>
+        <v>0.20663359683496854</v>
+      </c>
+    </row>
+    <row r="21" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F21">
         <v>84</v>
       </c>
@@ -777,14 +866,20 @@
         <f t="array" ref="G21">_xll.XLL.BLACK.PUT(f, sigma, F21, t)</f>
         <v>0.15048353300942807</v>
       </c>
-      <c r="H21" s="2"/>
+      <c r="H21" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F21,t)</f>
+        <v>0.17655906810759392</v>
+      </c>
       <c r="I21" cm="1">
         <f t="array" ref="I21">_xll.XLL.BLACK.PUT.IMPLIED(f, G21, F21, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J21" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H21, F21, t)</f>
+        <v>0.20623418333211044</v>
+      </c>
+    </row>
+    <row r="22" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F22">
         <v>85</v>
       </c>
@@ -792,14 +887,20 @@
         <f t="array" ref="G22">_xll.XLL.BLACK.PUT(f, sigma, F22, t)</f>
         <v>0.20168732797265232</v>
       </c>
-      <c r="H22" s="2"/>
+      <c r="H22" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F22,t)</f>
+        <v>0.23142008133591663</v>
+      </c>
       <c r="I22" cm="1">
         <f t="array" ref="I22">_xll.XLL.BLACK.PUT.IMPLIED(f, G22, F22, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J22" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H22, F22, t)</f>
+        <v>0.20583946803790867</v>
+      </c>
+    </row>
+    <row r="23" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F23">
         <v>86</v>
       </c>
@@ -807,14 +908,20 @@
         <f t="array" ref="G23">_xll.XLL.BLACK.PUT(f, sigma, F23, t)</f>
         <v>0.266480974586214</v>
       </c>
-      <c r="H23" s="2"/>
+      <c r="H23" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F23,t)</f>
+        <v>0.2997564826258321</v>
+      </c>
       <c r="I23" cm="1">
         <f t="array" ref="I23">_xll.XLL.BLACK.PUT.IMPLIED(f, G23, F23, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J23" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H23, F23, t)</f>
+        <v>0.20544934308943413</v>
+      </c>
+    </row>
+    <row r="24" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F24">
         <v>87</v>
       </c>
@@ -822,14 +929,20 @@
         <f t="array" ref="G24">_xll.XLL.BLACK.PUT(f, sigma, F24, t)</f>
         <v>0.34730740212793254</v>
       </c>
-      <c r="H24" s="2"/>
+      <c r="H24" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F24,t)</f>
+        <v>0.38385485890439863</v>
+      </c>
       <c r="I24" cm="1">
         <f t="array" ref="I24">_xll.XLL.BLACK.PUT.IMPLIED(f, G24, F24, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J24" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H24, F24, t)</f>
+        <v>0.20506370430575391</v>
+      </c>
+    </row>
+    <row r="25" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F25">
         <v>88</v>
       </c>
@@ -837,14 +950,20 @@
         <f t="array" ref="G25">_xll.XLL.BLACK.PUT(f, sigma, F25, t)</f>
         <v>0.44676133725329947</v>
       </c>
-      <c r="H25" s="2"/>
+      <c r="H25" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F25,t)</f>
+        <v>0.48614653111121164</v>
+      </c>
       <c r="I25" cm="1">
         <f t="array" ref="I25">_xll.XLL.BLACK.PUT.IMPLIED(f, G25, F25, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J25" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H25, F25, t)</f>
+        <v>0.20468245102133648</v>
+      </c>
+    </row>
+    <row r="26" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F26">
         <v>89</v>
       </c>
@@ -852,14 +971,20 @@
         <f t="array" ref="G26">_xll.XLL.BLACK.PUT(f, sigma, F26, t)</f>
         <v>0.56753930674006803</v>
       </c>
-      <c r="H26" s="2"/>
+      <c r="H26" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F26,t)</f>
+        <v>0.60916703344991596</v>
+      </c>
       <c r="I26" cm="1">
         <f t="array" ref="I26">_xll.XLL.BLACK.PUT.IMPLIED(f, G26, F26, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J26" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H26, F26, t)</f>
+        <v>0.20430548593030609</v>
+      </c>
+    </row>
+    <row r="27" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F27">
         <v>90</v>
       </c>
@@ -867,14 +992,20 @@
         <f t="array" ref="G27">_xll.XLL.BLACK.PUT(f, sigma, F27, t)</f>
         <v>0.71238089607367172</v>
       </c>
-      <c r="H27" s="2"/>
+      <c r="H27" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F27,t)</f>
+        <v>0.75550749047170562</v>
+      </c>
       <c r="I27" cm="1">
         <f t="array" ref="I27">_xll.XLL.BLACK.PUT.IMPLIED(f, G27, F27, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J27" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H27, F27, t)</f>
+        <v>0.20393271493704457</v>
+      </c>
+    </row>
+    <row r="28" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F28">
         <v>91</v>
       </c>
@@ -882,14 +1013,20 @@
         <f t="array" ref="G28">_xll.XLL.BLACK.PUT(f, sigma, F28, t)</f>
         <v>0.88400364647703356</v>
       </c>
-      <c r="H28" s="2"/>
+      <c r="H28" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F28,t)</f>
+        <v>0.92775945788765313</v>
+      </c>
       <c r="I28" cm="1">
         <f t="array" ref="I28">_xll.XLL.BLACK.PUT.IMPLIED(f, G28, F28, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J28" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H28, F28, t)</f>
+        <v>0.20356404701673117</v>
+      </c>
+    </row>
+    <row r="29" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F29">
         <v>92</v>
       </c>
@@ -897,14 +1034,20 @@
         <f t="array" ref="G29">_xll.XLL.BLACK.PUT(f, sigma, F29, t)</f>
         <v>1.0850344779622993</v>
       </c>
-      <c r="H29" s="2"/>
+      <c r="H29" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F29,t)</f>
+        <v>1.1284552798969685</v>
+      </c>
       <c r="I29" cm="1">
         <f t="array" ref="I29">_xll.XLL.BLACK.PUT.IMPLIED(f, G29, F29, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J29" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H29, F29, t)</f>
+        <v>0.20319939408279358</v>
+      </c>
+    </row>
+    <row r="30" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F30">
         <v>93</v>
       </c>
@@ -912,14 +1055,20 @@
         <f t="array" ref="G30">_xll.XLL.BLACK.PUT(f, sigma, F30, t)</f>
         <v>1.3179408286409853</v>
       </c>
-      <c r="H30" s="2"/>
+      <c r="H30" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F30,t)</f>
+        <v>1.360006387955174</v>
+      </c>
       <c r="I30" cm="1">
         <f t="array" ref="I30">_xll.XLL.BLACK.PUT.IMPLIED(f, G30, F30, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J30" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H30, F30, t)</f>
+        <v>0.20283867086138452</v>
+      </c>
+    </row>
+    <row r="31" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F31">
         <v>94</v>
       </c>
@@ -927,14 +1076,20 @@
         <f t="array" ref="G31">_xll.XLL.BLACK.PUT(f, sigma, F31, t)</f>
         <v>1.584964775689393</v>
       </c>
-      <c r="H31" s="2"/>
+      <c r="H31" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F31,t)</f>
+        <v>1.62464219013426</v>
+      </c>
       <c r="I31" cm="1">
         <f t="array" ref="I31">_xll.XLL.BLACK.PUT.IMPLIED(f, G31, F31, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J31" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H31, F31, t)</f>
+        <v>0.20248179477256115</v>
+      </c>
+    </row>
+    <row r="32" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F32">
         <v>95</v>
       </c>
@@ -942,14 +1097,20 @@
         <f t="array" ref="G32">_xll.XLL.BLACK.PUT(f, sigma, F32, t)</f>
         <v>1.8880632480607211</v>
       </c>
-      <c r="H32" s="2"/>
+      <c r="H32" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F32,t)</f>
+        <v>1.9243522559585848</v>
+      </c>
       <c r="I32" cm="1">
         <f t="array" ref="I32">_xll.XLL.BLACK.PUT.IMPLIED(f, G32, F32, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J32" s="2"/>
-    </row>
-    <row r="33" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J32" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H32, F32, t)</f>
+        <v>0.20212868581788687</v>
+      </c>
+    </row>
+    <row r="33" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F33">
         <v>96</v>
       </c>
@@ -957,14 +1118,20 @@
         <f t="array" ref="G33">_xll.XLL.BLACK.PUT(f, sigma, F33, t)</f>
         <v>2.2288570738163216</v>
       </c>
-      <c r="H33" s="2"/>
+      <c r="H33" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F33,t)</f>
+        <v>2.2608343827001036</v>
+      </c>
       <c r="I33" cm="1">
         <f t="array" ref="I33">_xll.XLL.BLACK.PUT.IMPLIED(f, G33, F33, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J33" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H33, F33, t)</f>
+        <v>0.20177926647365566</v>
+      </c>
+    </row>
+    <row r="34" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F34">
         <v>97</v>
       </c>
@@ -972,14 +1139,20 @@
         <f t="array" ref="G34">_xll.XLL.BLACK.PUT(f, sigma, F34, t)</f>
         <v>2.6085910627585847</v>
       </c>
-      <c r="H34" s="2"/>
+      <c r="H34" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F34,t)</f>
+        <v>2.6354508444062361</v>
+      </c>
       <c r="I34" cm="1">
         <f t="array" ref="I34">_xll.XLL.BLACK.PUT.IMPLIED(f, G34, F34, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J34" s="2"/>
-    </row>
-    <row r="35" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J34" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H34, F34, t)</f>
+        <v>0.20143346158876071</v>
+      </c>
+    </row>
+    <row r="35" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F35">
         <v>98</v>
       </c>
@@ -987,14 +1160,20 @@
         <f t="array" ref="G35">_xll.XLL.BLACK.PUT(f, sigma, F35, t)</f>
         <v>3.0281066582734937</v>
       </c>
-      <c r="H35" s="2"/>
+      <c r="H35" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F35,t)</f>
+        <v>3.0491946970869392</v>
+      </c>
       <c r="I35" cm="1">
         <f t="array" ref="I35">_xll.XLL.BLACK.PUT.IMPLIED(f, G35, F35, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J35" s="2"/>
-    </row>
-    <row r="36" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J35" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H35, F35, t)</f>
+        <v>0.20109119829026401</v>
+      </c>
+    </row>
+    <row r="36" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F36">
         <v>99</v>
       </c>
@@ -1002,14 +1181,20 @@
         <f t="array" ref="G36">_xll.XLL.BLACK.PUT(f, sigma, F36, t)</f>
         <v>3.4878279587501879</v>
       </c>
-      <c r="H36" s="2"/>
+      <c r="H36" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F36,t)</f>
+        <v>3.5026674760476624</v>
+      </c>
       <c r="I36" cm="1">
         <f t="array" ref="I36">_xll.XLL.BLACK.PUT.IMPLIED(f, G36, F36, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J36" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H36, F36, t)</f>
+        <v>0.20075240589094284</v>
+      </c>
+    </row>
+    <row r="37" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F37">
         <v>100</v>
       </c>
@@ -1017,14 +1202,20 @@
         <f t="array" ref="G37">_xll.XLL.BLACK.PUT(f, sigma, F37, t)</f>
         <v>3.987761167674492</v>
       </c>
-      <c r="H37" s="2"/>
+      <c r="H37" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F37,t)</f>
+        <v>3.9960690164368557</v>
+      </c>
       <c r="I37" cm="1">
         <f t="array" ref="I37">_xll.XLL.BLACK.PUT.IMPLIED(f, G37, F37, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J37" s="2"/>
-    </row>
-    <row r="38" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J37" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H37, F37, t)</f>
+        <v>0.20041701580256077</v>
+      </c>
+    </row>
+    <row r="38" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F38">
         <v>101</v>
       </c>
@@ -1032,14 +1223,20 @@
         <f t="array" ref="G38">_xll.XLL.BLACK.PUT(f, sigma, F38, t)</f>
         <v>4.5275068370385512</v>
       </c>
-      <c r="H38" s="2"/>
+      <c r="H38" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F38,t)</f>
+        <v>4.5291995002208836</v>
+      </c>
       <c r="I38" cm="1">
         <f t="array" ref="I38">_xll.XLL.BLACK.PUT.IMPLIED(f, G38, F38, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J38" s="2"/>
-    </row>
-    <row r="39" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J38" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H38, F38, t)</f>
+        <v>0.20008496145309618</v>
+      </c>
+    </row>
+    <row r="39" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F39">
         <v>102</v>
       </c>
@@ -1047,14 +1244,20 @@
         <f t="array" ref="G39">_xll.XLL.BLACK.PUT(f, sigma, F39, t)</f>
         <v>5.1062836665495652</v>
       </c>
-      <c r="H39" s="2"/>
+      <c r="H39" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F39,t)</f>
+        <v>5.1014732268873928</v>
+      </c>
       <c r="I39" cm="1">
         <f t="array" ref="I39">_xll.XLL.BLACK.PUT.IMPLIED(f, G39, F39, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J39" s="2"/>
-    </row>
-    <row r="40" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J39" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H39, F39, t)</f>
+        <v>0.19975617820979266</v>
+      </c>
+    </row>
+    <row r="40" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F40">
         <v>103</v>
       </c>
@@ -1062,14 +1265,20 @@
         <f t="array" ref="G40">_xll.XLL.BLACK.PUT(f, sigma, F40, t)</f>
         <v>5.7229621445706016</v>
       </c>
-      <c r="H40" s="2"/>
+      <c r="H40" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F40,t)</f>
+        <v>5.7119430607959316</v>
+      </c>
       <c r="I40" cm="1">
         <f t="array" ref="I40">_xll.XLL.BLACK.PUT.IMPLIED(f, G40, F40, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J40" s="2"/>
-    </row>
-    <row r="41" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J40" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H40, F40, t)</f>
+        <v>0.19943060330278106</v>
+      </c>
+    </row>
+    <row r="41" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F41">
         <v>104</v>
       </c>
@@ -1077,14 +1286,20 @@
         <f t="array" ref="G41">_xll.XLL.BLACK.PUT(f, sigma, F41, t)</f>
         <v>6.3761059854440632</v>
       </c>
-      <c r="H41" s="2"/>
+      <c r="H41" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F41,t)</f>
+        <v>6.359334058132589</v>
+      </c>
       <c r="I41" cm="1">
         <f t="array" ref="I41">_xll.XLL.BLACK.PUT.IMPLIED(f, G41, F41, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J41" s="2"/>
-    </row>
-    <row r="42" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J41" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H41, F41, t)</f>
+        <v>0.19910817575424916</v>
+      </c>
+    </row>
+    <row r="42" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F42">
         <v>105</v>
       </c>
@@ -1092,14 +1307,20 @@
         <f t="array" ref="G42">_xll.XLL.BLACK.PUT(f, sigma, F42, t)</f>
         <v>7.0640191378988533</v>
       </c>
-      <c r="H42" s="2"/>
+      <c r="H42" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F42,t)</f>
+        <v>7.0420844428201121</v>
+      </c>
       <c r="I42" cm="1">
         <f t="array" ref="I42">_xll.XLL.BLACK.PUT.IMPLIED(f, G42, F42, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J42" s="2"/>
-    </row>
-    <row r="43" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J42" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H42, F42, t)</f>
+        <v>0.19878883631142852</v>
+      </c>
+    </row>
+    <row r="43" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F43">
         <v>106</v>
       </c>
@@ -1107,14 +1328,20 @@
         <f t="array" ref="G43">_xll.XLL.BLACK.PUT(f, sigma, F43, t)</f>
         <v>7.7847961044341929</v>
       </c>
-      <c r="H43" s="2"/>
+      <c r="H43" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F43,t)</f>
+        <v>7.7583918958759028</v>
+      </c>
       <c r="I43" cm="1">
         <f t="array" ref="I43">_xll.XLL.BLACK.PUT.IMPLIED(f, G43, F43, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J43" s="2"/>
-    </row>
-    <row r="44" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J43" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H43, F43, t)</f>
+        <v>0.19847252738148907</v>
+      </c>
+    </row>
+    <row r="44" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F44">
         <v>107</v>
       </c>
@@ -1122,14 +1349,20 @@
         <f t="array" ref="G44">_xll.XLL.BLACK.PUT(f, sigma, F44, t)</f>
         <v>8.5363734057617648</v>
       </c>
-      <c r="H44" s="2"/>
+      <c r="H44" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F44,t)</f>
+        <v>8.5062630478467582</v>
+      </c>
       <c r="I44" cm="1">
         <f t="array" ref="I44">_xll.XLL.BLACK.PUT.IMPLIED(f, G44, F44, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J44" s="2"/>
-    </row>
-    <row r="45" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J44" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H44, F44, t)</f>
+        <v>0.19815919297022394</v>
+      </c>
+    </row>
+    <row r="45" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F45">
         <v>108</v>
       </c>
@@ -1137,14 +1370,20 @@
         <f t="array" ref="G45">_xll.XLL.BLACK.PUT(f, sigma, F45, t)</f>
         <v>9.3165802243033653</v>
       </c>
-      <c r="H45" s="2"/>
+      <c r="H45" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F45,t)</f>
+        <v>9.2835641106318576</v>
+      </c>
       <c r="I45" cm="1">
         <f t="array" ref="I45">_xll.XLL.BLACK.PUT.IMPLIED(f, G45, F45, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J45" s="2"/>
-    </row>
-    <row r="46" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J45" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H45, F45, t)</f>
+        <v>0.19784877862311953</v>
+      </c>
+    </row>
+    <row r="46" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F46">
         <v>109</v>
       </c>
@@ -1152,14 +1391,20 @@
         <f t="array" ref="G46">_xll.XLL.BLACK.PUT(f, sigma, F46, t)</f>
         <v>10.123186539019287</v>
       </c>
-      <c r="H46" s="2"/>
+      <c r="H46" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F46,t)</f>
+        <v>10.088070737440773</v>
+      </c>
       <c r="I46" cm="1">
         <f t="array" ref="I46">_xll.XLL.BLACK.PUT.IMPLIED(f, G46, F46, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J46" s="2"/>
-    </row>
-    <row r="47" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J46" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H46, F46, t)</f>
+        <v>0.19754123136892979</v>
+      </c>
+    </row>
+    <row r="47" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F47">
         <v>110</v>
       </c>
@@ -1167,14 +1412,20 @@
         <f t="array" ref="G47">_xll.XLL.BLACK.PUT(f, sigma, F47, t)</f>
         <v>10.953947391857227</v>
       </c>
-      <c r="H47" s="2"/>
+      <c r="H47" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F47,t)</f>
+        <v>10.917515436164138</v>
+      </c>
       <c r="I47" cm="1">
         <f t="array" ref="I47">_xll.XLL.BLACK.PUT.IMPLIED(f, G47, F47, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J47" s="2"/>
-    </row>
-    <row r="48" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J47" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H47, F47, t)</f>
+        <v>0.19723649966720683</v>
+      </c>
+    </row>
+    <row r="48" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F48">
         <v>111</v>
       </c>
@@ -1182,14 +1433,20 @@
         <f t="array" ref="G48">_xll.XLL.BLACK.PUT(f, sigma, F48, t)</f>
         <v>11.806642276452763</v>
       </c>
-      <c r="H48" s="2"/>
+      <c r="H48" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F48,t)</f>
+        <v>11.7696311573022</v>
+      </c>
       <c r="I48" cm="1">
         <f t="array" ref="I48">_xll.XLL.BLACK.PUT.IMPLIED(f, G48, F48, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J48" s="2"/>
-    </row>
-    <row r="49" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J48" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H48, F48, t)</f>
+        <v>0.19693453335599928</v>
+      </c>
+    </row>
+    <row r="49" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F49">
         <v>112</v>
       </c>
@@ -1197,14 +1454,20 @@
         <f t="array" ref="G49">_xll.XLL.BLACK.PUT(f, sigma, F49, t)</f>
         <v>12.679108988059141</v>
       </c>
-      <c r="H49" s="2"/>
+      <c r="H49" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F49,t)</f>
+        <v>12.64219000763228</v>
+      </c>
       <c r="I49" cm="1">
         <f t="array" ref="I49">_xll.XLL.BLACK.PUT.IMPLIED(f, G49, F49, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J49" s="2"/>
-    </row>
-    <row r="50" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J49" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H49, F49, t)</f>
+        <v>0.19663528360386642</v>
+      </c>
+    </row>
+    <row r="50" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F50">
         <v>113</v>
       </c>
@@ -1212,14 +1475,20 @@
         <f t="array" ref="G50">_xll.XLL.BLACK.PUT(f, sigma, F50, t)</f>
         <v>13.569271600088328</v>
       </c>
-      <c r="H50" s="2"/>
+      <c r="H50" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F50,t)</f>
+        <v>13.533036380390683</v>
+      </c>
       <c r="I50" cm="1">
         <f t="array" ref="I50">_xll.XLL.BLACK.PUT.IMPLIED(f, G50, F50, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J50" s="2"/>
-    </row>
-    <row r="51" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J50" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H50, F50, t)</f>
+        <v>0.19633870286258381</v>
+      </c>
+    </row>
+    <row r="51" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F51">
         <v>114</v>
       </c>
@@ -1227,14 +1496,20 @@
         <f t="array" ref="G51">_xll.XLL.BLACK.PUT(f, sigma, F51, t)</f>
         <v>14.47516252219144</v>
       </c>
-      <c r="H51" s="2"/>
+      <c r="H51" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F51,t)</f>
+        <v>14.44011412103788</v>
+      </c>
       <c r="I51" cm="1">
         <f t="array" ref="I51">_xll.XLL.BLACK.PUT.IMPLIED(f, G51, F51, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J51" s="2"/>
-    </row>
-    <row r="52" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J51" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H51, F51, t)</f>
+        <v>0.1960447448226682</v>
+      </c>
+    </row>
+    <row r="52" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F52">
         <v>115</v>
       </c>
@@ -1242,14 +1517,20 @@
         <f t="array" ref="G52">_xll.XLL.BLACK.PUT(f, sigma, F52, t)</f>
         <v>15.39493883771641</v>
       </c>
-      <c r="H52" s="2"/>
+      <c r="H52" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F52,t)</f>
+        <v>15.361487647106756</v>
+      </c>
       <c r="I52" cm="1">
         <f t="array" ref="I52">_xll.XLL.BLACK.PUT.IMPLIED(f, G52, F52, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J52" s="2"/>
-    </row>
-    <row r="53" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J52" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H52, F52, t)</f>
+        <v>0.19575336437070706</v>
+      </c>
+    </row>
+    <row r="53" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F53">
         <v>116</v>
       </c>
@@ -1257,14 +1538,20 @@
         <f t="array" ref="G53">_xll.XLL.BLACK.PUT(f, sigma, F53, t)</f>
         <v>16.32689330971084</v>
       </c>
-      <c r="H53" s="2"/>
+      <c r="H53" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F53,t)</f>
+        <v>16.29535719875858</v>
+      </c>
       <c r="I53" cm="1">
         <f t="array" ref="I53">_xll.XLL.BLACK.PUT.IMPLIED(f, G53, F53, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J53" s="2"/>
-    </row>
-    <row r="54" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J53" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H53, F53, t)</f>
+        <v>0.19546451754846336</v>
+      </c>
+    </row>
+    <row r="54" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F54">
         <v>117</v>
       </c>
@@ -1272,14 +1559,20 @@
         <f t="array" ref="G54">_xll.XLL.BLACK.PUT(f, sigma, F54, t)</f>
         <v>17.269460583629098</v>
       </c>
-      <c r="H54" s="2"/>
+      <c r="H54" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F54,t)</f>
+        <v>17.240068605568112</v>
+      </c>
       <c r="I54" cm="1">
         <f t="array" ref="I54">_xll.XLL.BLACK.PUT.IMPLIED(f, G54, F54, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J54" s="2"/>
-    </row>
-    <row r="55" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J54" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H54, F54, t)</f>
+        <v>0.19517816151349443</v>
+      </c>
+    </row>
+    <row r="55" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F55">
         <v>118</v>
       </c>
@@ -1287,14 +1580,20 @@
         <f t="array" ref="G55">_xll.XLL.BLACK.PUT(f, sigma, F55, t)</f>
         <v>18.221219204170339</v>
       </c>
-      <c r="H55" s="2"/>
+      <c r="H55" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F55,t)</f>
+        <v>18.194118111378401</v>
+      </c>
       <c r="I55" cm="1">
         <f t="array" ref="I55">_xll.XLL.BLACK.PUT.IMPLIED(f, G55, F55, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J55" s="2"/>
-    </row>
-    <row r="56" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J55" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H55, F55, t)</f>
+        <v>0.19489425450188741</v>
+      </c>
+    </row>
+    <row r="56" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F56">
         <v>119</v>
       </c>
@@ -1302,14 +1601,20 @@
         <f t="array" ref="G56">_xll.XLL.BLACK.PUT(f, sigma, F56, t)</f>
         <v>19.180890108309001</v>
       </c>
-      <c r="H56" s="2"/>
+      <c r="H56" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F56,t)</f>
+        <v>19.156152903317306</v>
+      </c>
       <c r="I56" cm="1">
         <f t="array" ref="I56">_xll.XLL.BLACK.PUT.IMPLIED(f, G56, F56, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J56" s="2"/>
-    </row>
-    <row r="57" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J56" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H56, F56, t)</f>
+        <v>0.1946127557918918</v>
+      </c>
+    </row>
+    <row r="57" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F57">
         <v>120</v>
       </c>
@@ -1317,14 +1622,20 @@
         <f t="array" ref="G57">_xll.XLL.BLACK.PUT(f, sigma, F57, t)</f>
         <v>20.14733226325697</v>
       </c>
-      <c r="H57" s="2"/>
+      <c r="H57" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F57,t)</f>
+        <v>20.12496804698003</v>
+      </c>
       <c r="I57" cm="1">
         <f t="array" ref="I57">_xll.XLL.BLACK.PUT.IMPLIED(f, G57, F57, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J57" s="2"/>
-    </row>
-    <row r="58" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J57" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H57, F57, t)</f>
+        <v>0.19433362566998369</v>
+      </c>
+    </row>
+    <row r="58" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F58">
         <v>121</v>
       </c>
@@ -1332,14 +1643,20 @@
         <f t="array" ref="G58">_xll.XLL.BLACK.PUT(f, sigma, F58, t)</f>
         <v>21.119536094302745</v>
       </c>
-      <c r="H58" s="2"/>
+      <c r="H58" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F58,t)</f>
+        <v>21.099500543233205</v>
+      </c>
       <c r="I58" cm="1">
         <f t="array" ref="I58">_xll.XLL.BLACK.PUT.IMPLIED(f, G58, F58, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J58" s="2"/>
-    </row>
-    <row r="59" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J58" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H58, F58, t)</f>
+        <v>0.19405682539738733</v>
+      </c>
+    </row>
+    <row r="59" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F59">
         <v>122</v>
       </c>
@@ -1347,14 +1664,20 @@
         <f t="array" ref="G59">_xll.XLL.BLACK.PUT(f, sigma, F59, t)</f>
         <v>22.096615300806519</v>
       </c>
-      <c r="H59" s="2"/>
+      <c r="H59" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F59,t)</f>
+        <v>22.078821200533753</v>
+      </c>
       <c r="I59" cm="1">
         <f t="array" ref="I59">_xll.XLL.BLACK.PUT.IMPLIED(f, G59, F59, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J59" s="2"/>
-    </row>
-    <row r="60" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J59" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H59, F59, t)</f>
+        <v>0.19378231717859215</v>
+      </c>
+    </row>
+    <row r="60" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F60">
         <v>123</v>
       </c>
@@ -1362,14 +1685,20 @@
         <f t="array" ref="G60">_xll.XLL.BLACK.PUT(f, sigma, F60, t)</f>
         <v>23.077797596311726</v>
       </c>
-      <c r="H60" s="2"/>
+      <c r="H60" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F60,t)</f>
+        <v>23.062124968007112</v>
+      </c>
       <c r="I60" cm="1">
         <f t="array" ref="I60">_xll.XLL.BLACK.PUT.IMPLIED(f, G60, F60, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J60" s="2"/>
-    </row>
-    <row r="61" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J60" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H60, F60, t)</f>
+        <v>0.19351006413067628</v>
+      </c>
+    </row>
+    <row r="61" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F61">
         <v>124</v>
       </c>
@@ -1377,14 +1706,20 @@
         <f t="array" ref="G61">_xll.XLL.BLACK.PUT(f, sigma, F61, t)</f>
         <v>24.062414837222818</v>
       </c>
-      <c r="H61" s="2"/>
+      <c r="H61" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F61,t)</f>
+        <v>24.04872030681635</v>
+      </c>
       <c r="I61" cm="1">
         <f t="array" ref="I61">_xll.XLL.BLACK.PUT.IMPLIED(f, G61, F61, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J61" s="2"/>
-    </row>
-    <row r="62" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J61" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H61, F61, t)</f>
+        <v>0.19324003025443812</v>
+      </c>
+    </row>
+    <row r="62" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F62">
         <v>125</v>
       </c>
@@ -1392,14 +1727,20 @@
         <f t="array" ref="G62">_xll.XLL.BLACK.PUT(f, sigma, F62, t)</f>
         <v>25.04989292927732</v>
       </c>
-      <c r="H62" s="2"/>
+      <c r="H62" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F62,t)</f>
+        <v>25.038018097943663</v>
+      </c>
       <c r="I62" cm="1">
         <f t="array" ref="I62">_xll.XLL.BLACK.PUT.IMPLIED(f, G62, F62, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J62" s="2"/>
-    </row>
-    <row r="63" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J62" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H62, F62, t)</f>
+        <v>0.19297218040625874</v>
+      </c>
+    </row>
+    <row r="63" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F63">
         <v>126</v>
       </c>
@@ -1407,14 +1748,20 @@
         <f t="array" ref="G63">_xll.XLL.BLACK.PUT(f, sigma, F63, t)</f>
         <v>26.039741826510507</v>
       </c>
-      <c r="H63" s="2"/>
+      <c r="H63" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F63,t)</f>
+        <v>26.029520499927315</v>
+      </c>
       <c r="I63" cm="1">
         <f t="array" ref="I63">_xll.XLL.BLACK.PUT.IMPLIED(f, G63, F63, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J63" s="2"/>
-    </row>
-    <row r="64" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J63" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H63, F63, t)</f>
+        <v>0.19270648027075188</v>
+      </c>
+    </row>
+    <row r="64" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F64">
         <v>127</v>
       </c>
@@ -1422,14 +1769,20 @@
         <f t="array" ref="G64">_xll.XLL.BLACK.PUT(f, sigma, F64, t)</f>
         <v>27.031545866893069</v>
       </c>
-      <c r="H64" s="2"/>
+      <c r="H64" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F64,t)</f>
+        <v>27.022810085691404</v>
+      </c>
       <c r="I64" cm="1">
         <f t="array" ref="I64">_xll.XLL.BLACK.PUT.IMPLIED(f, G64, F64, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J64" s="2"/>
-    </row>
-    <row r="65" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J64" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H64, F64, t)</f>
+        <v>0.19244289633549364</v>
+      </c>
+    </row>
+    <row r="65" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F65">
         <v>128</v>
       </c>
@@ -1437,14 +1790,20 @@
         <f t="array" ref="G65">_xll.XLL.BLACK.PUT(f, sigma, F65, t)</f>
         <v>28.024954624625238</v>
       </c>
-      <c r="H65" s="2"/>
+      <c r="H65" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F65,t)</f>
+        <v>28.017539507525299</v>
+      </c>
       <c r="I65" cm="1">
         <f t="array" ref="I65">_xll.XLL.BLACK.PUT.IMPLIED(f, G65, F65, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J65" s="2"/>
-    </row>
-    <row r="66" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J65" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H65, F65, t)</f>
+        <v>0.19218139586568742</v>
+      </c>
+    </row>
+    <row r="66" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F66">
         <v>129</v>
       </c>
@@ -1452,14 +1811,20 @@
         <f t="array" ref="G66">_xll.XLL.BLACK.PUT(f, sigma, F66, t)</f>
         <v>29.01967440261366</v>
       </c>
-      <c r="H66" s="2"/>
+      <c r="H66" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F66,t)</f>
+        <v>29.013421866483313</v>
+      </c>
       <c r="I66" cm="1">
         <f t="array" ref="I66">_xll.XLL.BLACK.PUT.IMPLIED(f, G66, F66, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J66" s="2"/>
-    </row>
-    <row r="67" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J66" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H66, F66, t)</f>
+        <v>0.19192194688040323</v>
+      </c>
+    </row>
+    <row r="67" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F67">
         <v>130</v>
       </c>
@@ -1467,12 +1832,18 @@
         <f t="array" ref="G67">_xll.XLL.BLACK.PUT(f, sigma, F67, t)</f>
         <v>30.01546044060332</v>
       </c>
-      <c r="H67" s="2"/>
+      <c r="H67" s="2">
+        <f>_xll.XLL.GAMMA.PUT(f,sigma,F67,t)</f>
+        <v>30.010221898820959</v>
+      </c>
       <c r="I67" cm="1">
         <f t="array" ref="I67">_xll.XLL.BLACK.PUT.IMPLIED(f, G67, F67, t)</f>
         <v>0.2</v>
       </c>
-      <c r="J67" s="2"/>
+      <c r="J67" s="2">
+        <f>_xll.XLL.BLACK.PUT.IMPLIED(f, H67, F67, t)</f>
+        <v>0.19166451812980059</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>